<commit_message>
Adding data to charts
</commit_message>
<xml_diff>
--- a/mem-test/snapshots/v1.5.8/03-init-connections-2/memory-log.xlsx
+++ b/mem-test/snapshots/v1.5.8/03-init-connections-2/memory-log.xlsx
@@ -212,11 +212,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -232,6 +233,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -353,12 +364,40 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>03 - init connections</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -409,6 +448,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -641,6 +681,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -873,6 +914,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1105,6 +1147,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1337,6 +1380,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1531,17 +1575,17 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="17849656"/>
-        <c:axId val="47674210"/>
+        <c:axId val="64466065"/>
+        <c:axId val="88229125"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="17849656"/>
+        <c:axId val="64466065"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1563,7 +1607,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47674210"/>
+        <c:crossAx val="88229125"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1571,7 +1615,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47674210"/>
+        <c:axId val="88229125"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1586,7 +1630,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1608,7 +1652,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17849656"/>
+        <c:crossAx val="64466065"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1667,9 +1711,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>403200</xdr:colOff>
+      <xdr:colOff>402840</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1677,8 +1721,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7686360" y="153000"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="7687440" y="153000"/>
+        <a:ext cx="5768640" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1699,14 +1743,14 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+      <selection pane="topLeft" activeCell="K26" activeCellId="0" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.74"/>

</xml_diff>